<commit_message>
added xlabel to plot in monte carlo GUI
</commit_message>
<xml_diff>
--- a/MATLAB/results_montecarlo.xlsx
+++ b/MATLAB/results_montecarlo.xlsx
@@ -435,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A3" sqref="A3:T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,6 +505,130 @@
         <v>19</v>
       </c>
     </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.04</v>
+      </c>
+      <c r="K2">
+        <v>0.04</v>
+      </c>
+      <c r="L2">
+        <v>0.04</v>
+      </c>
+      <c r="M2">
+        <v>0.04</v>
+      </c>
+      <c r="N2">
+        <v>200</v>
+      </c>
+      <c r="O2">
+        <v>300</v>
+      </c>
+      <c r="P2">
+        <v>600</v>
+      </c>
+      <c r="Q2">
+        <v>0.15049296094977052</v>
+      </c>
+      <c r="R2">
+        <v>1.3721046507395801E-3</v>
+      </c>
+      <c r="S2">
+        <v>0.3480414117524081</v>
+      </c>
+      <c r="T2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.04</v>
+      </c>
+      <c r="K3">
+        <v>0.04</v>
+      </c>
+      <c r="L3">
+        <v>0.04</v>
+      </c>
+      <c r="M3">
+        <v>0.04</v>
+      </c>
+      <c r="N3">
+        <v>200</v>
+      </c>
+      <c r="O3">
+        <v>300</v>
+      </c>
+      <c r="P3">
+        <v>600</v>
+      </c>
+      <c r="Q3">
+        <v>0.19161495366676654</v>
+      </c>
+      <c r="R3">
+        <v>1.2558213135784916E-3</v>
+      </c>
+      <c r="S3">
+        <v>0.33438156265954805</v>
+      </c>
+      <c r="T3">
+        <v>10000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added iterations field in data tuple and fixed excel write issue
</commit_message>
<xml_diff>
--- a/MATLAB/results_montecarlo.xlsx
+++ b/MATLAB/results_montecarlo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Speed</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>Iterations</t>
+  </si>
+  <si>
+    <t>Arrivals</t>
+  </si>
+  <si>
+    <t>Lead Time Requirement</t>
+  </si>
+  <si>
+    <t>Idle Time Requirement</t>
   </si>
 </sst>
 </file>
@@ -435,15 +444,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:T3"/>
+      <selection activeCell="A2" sqref="A2:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,10 +514,22 @@
         <v>17</v>
       </c>
       <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
         <v>19</v>
       </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.9000000000000004</v>
       </c>
@@ -555,78 +579,28 @@
         <v>600</v>
       </c>
       <c r="Q2">
-        <v>0.15049296094977052</v>
+        <v>0.16961226948758149</v>
       </c>
       <c r="R2">
-        <v>1.3721046507395801E-3</v>
+        <v>1.7034686872567876E-2</v>
       </c>
       <c r="S2">
-        <v>0.3480414117524081</v>
+        <v>0.33569177934307826</v>
       </c>
       <c r="T2">
+        <v>4.5314641980172569E-3</v>
+      </c>
+      <c r="U2">
         <v>10000</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>16</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0.04</v>
-      </c>
-      <c r="K3">
-        <v>0.04</v>
-      </c>
-      <c r="L3">
-        <v>0.04</v>
-      </c>
-      <c r="M3">
-        <v>0.04</v>
-      </c>
-      <c r="N3">
-        <v>200</v>
-      </c>
-      <c r="O3">
-        <v>300</v>
-      </c>
-      <c r="P3">
-        <v>600</v>
-      </c>
-      <c r="Q3">
-        <v>0.19161495366676654</v>
-      </c>
-      <c r="R3">
-        <v>1.2558213135784916E-3</v>
-      </c>
-      <c r="S3">
-        <v>0.33438156265954805</v>
-      </c>
-      <c r="T3">
-        <v>10000</v>
+      <c r="V2">
+        <v>5</v>
+      </c>
+      <c r="W2">
+        <v>0.5</v>
+      </c>
+      <c r="X2">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the save results function
</commit_message>
<xml_diff>
--- a/MATLAB/results_montecarlo.xlsx
+++ b/MATLAB/results_montecarlo.xlsx
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:X2"/>
+      <selection activeCell="A5" sqref="A5:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,6 +603,192 @@
         <v>50</v>
       </c>
     </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.04</v>
+      </c>
+      <c r="K3">
+        <v>0.04</v>
+      </c>
+      <c r="L3">
+        <v>0.04</v>
+      </c>
+      <c r="M3">
+        <v>0.04</v>
+      </c>
+      <c r="N3">
+        <v>200</v>
+      </c>
+      <c r="O3">
+        <v>300</v>
+      </c>
+      <c r="P3">
+        <v>600</v>
+      </c>
+      <c r="Q3">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="R3">
+        <v>0.33</v>
+      </c>
+      <c r="S3">
+        <v>0.5</v>
+      </c>
+      <c r="T3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.04</v>
+      </c>
+      <c r="K4">
+        <v>0.04</v>
+      </c>
+      <c r="L4">
+        <v>0.04</v>
+      </c>
+      <c r="M4">
+        <v>0.04</v>
+      </c>
+      <c r="N4">
+        <v>200</v>
+      </c>
+      <c r="O4">
+        <v>300</v>
+      </c>
+      <c r="P4">
+        <v>600</v>
+      </c>
+      <c r="Q4">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="R4">
+        <v>0.33</v>
+      </c>
+      <c r="S4">
+        <v>0.5</v>
+      </c>
+      <c r="T4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.04</v>
+      </c>
+      <c r="K5">
+        <v>0.04</v>
+      </c>
+      <c r="L5">
+        <v>0.04</v>
+      </c>
+      <c r="M5">
+        <v>0.04</v>
+      </c>
+      <c r="N5">
+        <v>200</v>
+      </c>
+      <c r="O5">
+        <v>300</v>
+      </c>
+      <c r="P5">
+        <v>600</v>
+      </c>
+      <c r="Q5">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="R5">
+        <v>0.33</v>
+      </c>
+      <c r="S5">
+        <v>0.5</v>
+      </c>
+      <c r="T5">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
monte carlo results and sensitivity analysis added
</commit_message>
<xml_diff>
--- a/MATLAB/results_montecarlo.xlsx
+++ b/MATLAB/results_montecarlo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,6 +530,1162 @@
         <v>22</v>
       </c>
     </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.04</v>
+      </c>
+      <c r="K2">
+        <v>0.04</v>
+      </c>
+      <c r="L2">
+        <v>0.04</v>
+      </c>
+      <c r="M2">
+        <v>0.04</v>
+      </c>
+      <c r="N2">
+        <v>50</v>
+      </c>
+      <c r="O2">
+        <v>200</v>
+      </c>
+      <c r="P2">
+        <v>550</v>
+      </c>
+      <c r="Q2">
+        <v>2.6778146297450366E-2</v>
+      </c>
+      <c r="R2">
+        <v>4.3962823000668649E-5</v>
+      </c>
+      <c r="S2">
+        <v>0.75059218247115644</v>
+      </c>
+      <c r="T2">
+        <v>7.6075678035148722E-4</v>
+      </c>
+      <c r="U2">
+        <v>10000</v>
+      </c>
+      <c r="V2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.04</v>
+      </c>
+      <c r="K3">
+        <v>0.04</v>
+      </c>
+      <c r="L3">
+        <v>0.04</v>
+      </c>
+      <c r="M3">
+        <v>0.04</v>
+      </c>
+      <c r="N3">
+        <v>50</v>
+      </c>
+      <c r="O3">
+        <v>200</v>
+      </c>
+      <c r="P3">
+        <v>650</v>
+      </c>
+      <c r="Q3">
+        <v>2.6359855079758819E-2</v>
+      </c>
+      <c r="R3">
+        <v>6.5516638209457519E-5</v>
+      </c>
+      <c r="S3">
+        <v>0.75270689500497256</v>
+      </c>
+      <c r="T3">
+        <v>1.231052177134672E-3</v>
+      </c>
+      <c r="U3">
+        <v>10000</v>
+      </c>
+      <c r="V3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.04</v>
+      </c>
+      <c r="K4">
+        <v>0.04</v>
+      </c>
+      <c r="L4">
+        <v>0.04</v>
+      </c>
+      <c r="M4">
+        <v>0.04</v>
+      </c>
+      <c r="N4">
+        <v>50</v>
+      </c>
+      <c r="O4">
+        <v>400</v>
+      </c>
+      <c r="P4">
+        <v>550</v>
+      </c>
+      <c r="Q4">
+        <v>2.0550519571121802E-2</v>
+      </c>
+      <c r="R4">
+        <v>1.6755811335919091E-5</v>
+      </c>
+      <c r="S4">
+        <v>0.87568495429540083</v>
+      </c>
+      <c r="T4">
+        <v>7.8245972291806948E-4</v>
+      </c>
+      <c r="U4">
+        <v>10000</v>
+      </c>
+      <c r="V4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.04</v>
+      </c>
+      <c r="K5">
+        <v>0.04</v>
+      </c>
+      <c r="L5">
+        <v>0.04</v>
+      </c>
+      <c r="M5">
+        <v>0.04</v>
+      </c>
+      <c r="N5">
+        <v>50</v>
+      </c>
+      <c r="O5">
+        <v>400</v>
+      </c>
+      <c r="P5">
+        <v>650</v>
+      </c>
+      <c r="Q5">
+        <v>2.0245401844702294E-2</v>
+      </c>
+      <c r="R5">
+        <v>1.7154700252746717E-5</v>
+      </c>
+      <c r="S5">
+        <v>0.87497537994888508</v>
+      </c>
+      <c r="T5">
+        <v>4.5083352932814543E-4</v>
+      </c>
+      <c r="U5">
+        <v>10000</v>
+      </c>
+      <c r="V5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0.04</v>
+      </c>
+      <c r="K6">
+        <v>0.04</v>
+      </c>
+      <c r="L6">
+        <v>0.04</v>
+      </c>
+      <c r="M6">
+        <v>0.04</v>
+      </c>
+      <c r="N6">
+        <v>150</v>
+      </c>
+      <c r="O6">
+        <v>200</v>
+      </c>
+      <c r="P6">
+        <v>550</v>
+      </c>
+      <c r="Q6">
+        <v>4.3957818870319264E-2</v>
+      </c>
+      <c r="R6">
+        <v>7.9814966304870704E-4</v>
+      </c>
+      <c r="S6">
+        <v>0.25194706997238797</v>
+      </c>
+      <c r="T6">
+        <v>6.1224566195884674E-3</v>
+      </c>
+      <c r="U6">
+        <v>10000</v>
+      </c>
+      <c r="V6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0.04</v>
+      </c>
+      <c r="K7">
+        <v>0.04</v>
+      </c>
+      <c r="L7">
+        <v>0.04</v>
+      </c>
+      <c r="M7">
+        <v>0.04</v>
+      </c>
+      <c r="N7">
+        <v>150</v>
+      </c>
+      <c r="O7">
+        <v>200</v>
+      </c>
+      <c r="P7">
+        <v>650</v>
+      </c>
+      <c r="Q7">
+        <v>4.4538518109261356E-2</v>
+      </c>
+      <c r="R7">
+        <v>7.0767034001242661E-4</v>
+      </c>
+      <c r="S7">
+        <v>0.24598611452073321</v>
+      </c>
+      <c r="T7">
+        <v>6.5058650103057203E-3</v>
+      </c>
+      <c r="U7">
+        <v>10000</v>
+      </c>
+      <c r="V7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0.04</v>
+      </c>
+      <c r="K8">
+        <v>0.04</v>
+      </c>
+      <c r="L8">
+        <v>0.04</v>
+      </c>
+      <c r="M8">
+        <v>0.04</v>
+      </c>
+      <c r="N8">
+        <v>150</v>
+      </c>
+      <c r="O8">
+        <v>400</v>
+      </c>
+      <c r="P8">
+        <v>550</v>
+      </c>
+      <c r="Q8">
+        <v>2.7815436958749711E-2</v>
+      </c>
+      <c r="R8">
+        <v>2.1681259332896008E-4</v>
+      </c>
+      <c r="S8">
+        <v>0.62929472625482163</v>
+      </c>
+      <c r="T8">
+        <v>1.8967545717024918E-3</v>
+      </c>
+      <c r="U8">
+        <v>10000</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0.04</v>
+      </c>
+      <c r="K9">
+        <v>0.04</v>
+      </c>
+      <c r="L9">
+        <v>0.04</v>
+      </c>
+      <c r="M9">
+        <v>0.04</v>
+      </c>
+      <c r="N9">
+        <v>150</v>
+      </c>
+      <c r="O9">
+        <v>400</v>
+      </c>
+      <c r="P9">
+        <v>650</v>
+      </c>
+      <c r="Q9">
+        <v>2.7674836447346463E-2</v>
+      </c>
+      <c r="R9">
+        <v>1.9194458530667486E-4</v>
+      </c>
+      <c r="S9">
+        <v>0.6245760128162916</v>
+      </c>
+      <c r="T9">
+        <v>1.5083122669846891E-3</v>
+      </c>
+      <c r="U9">
+        <v>10000</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0.02</v>
+      </c>
+      <c r="K10">
+        <v>0.02</v>
+      </c>
+      <c r="L10">
+        <v>0.02</v>
+      </c>
+      <c r="M10">
+        <v>0.02</v>
+      </c>
+      <c r="N10">
+        <v>50</v>
+      </c>
+      <c r="O10">
+        <v>200</v>
+      </c>
+      <c r="P10">
+        <v>550</v>
+      </c>
+      <c r="Q10">
+        <v>2.4539692177653512E-2</v>
+      </c>
+      <c r="R10">
+        <v>2.1646434886623961E-5</v>
+      </c>
+      <c r="S10">
+        <v>0.75037632108335739</v>
+      </c>
+      <c r="T10">
+        <v>1.3343137874497455E-3</v>
+      </c>
+      <c r="U10">
+        <v>10000</v>
+      </c>
+      <c r="V10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0.02</v>
+      </c>
+      <c r="K11">
+        <v>0.02</v>
+      </c>
+      <c r="L11">
+        <v>0.02</v>
+      </c>
+      <c r="M11">
+        <v>0.02</v>
+      </c>
+      <c r="N11">
+        <v>50</v>
+      </c>
+      <c r="O11">
+        <v>200</v>
+      </c>
+      <c r="P11">
+        <v>650</v>
+      </c>
+      <c r="Q11">
+        <v>2.4213497869152573E-2</v>
+      </c>
+      <c r="R11">
+        <v>5.8184315360275055E-5</v>
+      </c>
+      <c r="S11">
+        <v>0.74992873058871601</v>
+      </c>
+      <c r="T11">
+        <v>1.6374346347852624E-3</v>
+      </c>
+      <c r="U11">
+        <v>10000</v>
+      </c>
+      <c r="V11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0.02</v>
+      </c>
+      <c r="K12">
+        <v>0.02</v>
+      </c>
+      <c r="L12">
+        <v>0.02</v>
+      </c>
+      <c r="M12">
+        <v>0.02</v>
+      </c>
+      <c r="N12">
+        <v>50</v>
+      </c>
+      <c r="O12">
+        <v>400</v>
+      </c>
+      <c r="P12">
+        <v>550</v>
+      </c>
+      <c r="Q12">
+        <v>1.8240823472723662E-2</v>
+      </c>
+      <c r="R12">
+        <v>4.9349792156898743E-5</v>
+      </c>
+      <c r="S12">
+        <v>0.87563652501947487</v>
+      </c>
+      <c r="T12">
+        <v>8.5836951990923946E-4</v>
+      </c>
+      <c r="U12">
+        <v>10000</v>
+      </c>
+      <c r="V12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0.02</v>
+      </c>
+      <c r="K13">
+        <v>0.02</v>
+      </c>
+      <c r="L13">
+        <v>0.02</v>
+      </c>
+      <c r="M13">
+        <v>0.02</v>
+      </c>
+      <c r="N13">
+        <v>50</v>
+      </c>
+      <c r="O13">
+        <v>400</v>
+      </c>
+      <c r="P13">
+        <v>650</v>
+      </c>
+      <c r="Q13">
+        <v>1.7879609926206443E-2</v>
+      </c>
+      <c r="R13">
+        <v>1.183869852412298E-5</v>
+      </c>
+      <c r="S13">
+        <v>0.8763785555182082</v>
+      </c>
+      <c r="T13">
+        <v>4.9796300225006442E-4</v>
+      </c>
+      <c r="U13">
+        <v>10000</v>
+      </c>
+      <c r="V13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0.02</v>
+      </c>
+      <c r="K14">
+        <v>0.02</v>
+      </c>
+      <c r="L14">
+        <v>0.02</v>
+      </c>
+      <c r="M14">
+        <v>0.02</v>
+      </c>
+      <c r="N14">
+        <v>150</v>
+      </c>
+      <c r="O14">
+        <v>200</v>
+      </c>
+      <c r="P14">
+        <v>550</v>
+      </c>
+      <c r="Q14">
+        <v>3.9892509643641903E-2</v>
+      </c>
+      <c r="R14">
+        <v>1.1825732614869787E-3</v>
+      </c>
+      <c r="S14">
+        <v>0.25628908681405488</v>
+      </c>
+      <c r="T14">
+        <v>6.9030646042207953E-3</v>
+      </c>
+      <c r="U14">
+        <v>10000</v>
+      </c>
+      <c r="V14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0.02</v>
+      </c>
+      <c r="K15">
+        <v>0.02</v>
+      </c>
+      <c r="L15">
+        <v>0.02</v>
+      </c>
+      <c r="M15">
+        <v>0.02</v>
+      </c>
+      <c r="N15">
+        <v>150</v>
+      </c>
+      <c r="O15">
+        <v>200</v>
+      </c>
+      <c r="P15">
+        <v>650</v>
+      </c>
+      <c r="Q15">
+        <v>3.9516862894926383E-2</v>
+      </c>
+      <c r="R15">
+        <v>6.0546006907180778E-4</v>
+      </c>
+      <c r="S15">
+        <v>0.24213908670634252</v>
+      </c>
+      <c r="T15">
+        <v>3.793029428375587E-3</v>
+      </c>
+      <c r="U15">
+        <v>10000</v>
+      </c>
+      <c r="V15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0.02</v>
+      </c>
+      <c r="K16">
+        <v>0.02</v>
+      </c>
+      <c r="L16">
+        <v>0.02</v>
+      </c>
+      <c r="M16">
+        <v>0.02</v>
+      </c>
+      <c r="N16">
+        <v>150</v>
+      </c>
+      <c r="O16">
+        <v>400</v>
+      </c>
+      <c r="P16">
+        <v>550</v>
+      </c>
+      <c r="Q16">
+        <v>2.2133205741508073E-2</v>
+      </c>
+      <c r="R16">
+        <v>5.0734586515548537E-5</v>
+      </c>
+      <c r="S16">
+        <v>0.62495074185562127</v>
+      </c>
+      <c r="T16">
+        <v>1.1058087229678692E-3</v>
+      </c>
+      <c r="U16">
+        <v>10000</v>
+      </c>
+      <c r="V16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0.02</v>
+      </c>
+      <c r="K17">
+        <v>0.02</v>
+      </c>
+      <c r="L17">
+        <v>0.02</v>
+      </c>
+      <c r="M17">
+        <v>0.02</v>
+      </c>
+      <c r="N17">
+        <v>150</v>
+      </c>
+      <c r="O17">
+        <v>400</v>
+      </c>
+      <c r="P17">
+        <v>650</v>
+      </c>
+      <c r="Q17">
+        <v>2.1624865597261064E-2</v>
+      </c>
+      <c r="R17">
+        <v>1.3106489658985156E-4</v>
+      </c>
+      <c r="S17">
+        <v>0.62564164592989302</v>
+      </c>
+      <c r="T17">
+        <v>2.4818793314518692E-3</v>
+      </c>
+      <c r="U17">
+        <v>10000</v>
+      </c>
+      <c r="V17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0.03</v>
+      </c>
+      <c r="K18">
+        <v>0.03</v>
+      </c>
+      <c r="L18">
+        <v>0.03</v>
+      </c>
+      <c r="M18">
+        <v>0.03</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
+      </c>
+      <c r="O18">
+        <v>300</v>
+      </c>
+      <c r="P18">
+        <v>600</v>
+      </c>
+      <c r="Q18">
+        <v>2.3352437180671114E-2</v>
+      </c>
+      <c r="R18">
+        <v>6.9821935068287361E-5</v>
+      </c>
+      <c r="S18">
+        <v>0.66408766945349051</v>
+      </c>
+      <c r="T18">
+        <v>1.4568814848845209E-3</v>
+      </c>
+      <c r="U18">
+        <v>10000</v>
+      </c>
+      <c r="V18">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -540,7 +1696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B57E2A-D555-4FF2-A876-71EC879364D8}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>

</xml_diff>